<commit_message>
add more strings to db
</commit_message>
<xml_diff>
--- a/files/strings.xlsx
+++ b/files/strings.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/storex/dLab/andStudio/lime-strings/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C28BAD2D-8662-724E-BE79-44608F4F1ADE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00699DF6-3001-3C41-88D7-47BE962DB03C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{2A2A4A0D-8F67-1149-8B79-481C2E1F4E29}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="3" xr2:uid="{2A2A4A0D-8F67-1149-8B79-481C2E1F4E29}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1260" uniqueCount="924">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1306" uniqueCount="970">
   <si>
     <t>bangla</t>
   </si>
@@ -2804,6 +2805,2904 @@
   </si>
   <si>
     <t>ভিডিও পাওয়া নি</t>
+  </si>
+  <si>
+    <r>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">string </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>name</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF008000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>="movies"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt;সিনেমা&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>string</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">string </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>name</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF008000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>="drama"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt;নাটক&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>string</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">string </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>name</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF008000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>="tv_shows"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt;টিভি শো&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>string</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">string </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>name</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF008000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>="sports"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt;খেলাধুলা&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>string</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">string </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>name</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF008000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>="more"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt;আরও&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>string</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">string </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>name</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF008000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>="my_profile"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt;আমার প্রোফাইল&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>string</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">string </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>name</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF008000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>="we_encountered_an_expected_pb"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt;দুঃখিত, কোন অনাকাংখিত সমস্যা হয়েছে&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>string</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">string </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>name</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF008000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>="invite_friends"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt;ফ্রেন্ডদের ইনভাইট করুন&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>string</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">string </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>name</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF008000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>="notification_settings"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt;নোটিফিকেশন সেটিংস&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>string</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">string </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>name</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF008000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>="description"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt;বিস্তারিত&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>string</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">string </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>name</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF008000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>="permission_gallery"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt;আপনার প্রোফাইল পেইজে ছবি আপলোড করার জন্য দয়া করে বায়স্কোপকে আপনার ডিভাইসের ছবি এবং মিডিয়া ফাইলস এক্সেস করার অনুমতি দিন&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>string</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">string </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>name</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF008000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>="confirmation_sign_out"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt;আপনি কি বায়স্কোপ থেকে সাইন আউট করতে চান?&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>string</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">string </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>name</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF008000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>="not_found"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt;কোন প্রিয় আইটেম নেই&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>string</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">string </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>name</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF008000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>="msg_subscription_trial_ending"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt;আর মাত্র %s দিন বাকি, আপনাার %s শেষ হবার। বায়োস্কোপ উপভোগ করার জন্য যে কোন একটি প্রিমিয়াম প্ল্যান এ সাবস্ক্রাইব করুন।&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>string</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">string </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>name</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF008000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>="your_subscription_will_not_be_auto_renewed"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt;অটো নবায়ন করা হবে না&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>string</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">string </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>name</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF008000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>="your_subscription_will_not_be_automatically_renewed_in_the_next_cycle"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt;পরবর্তি বিলিং সাইকেলে আপনার সাবস্ক্রিপশন অটো নবায়ন করা হবে না&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>string</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">string </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>name</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF008000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>="your_subscription_will_be_auto_renewed"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt;আপনার সাবস্ক্রিপশন স্বয়ংক্রিয়ভাবে পুনঃ নবায়ন হবে&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>string</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">string </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>name</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF008000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>="your_subscription_will_be_automatically_renewed_in_the_next_cycle"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt;আপনার সাবস্ক্রিপশন পরবর্তী চক্রে স্বয়ংক্রিয়ভাবে পুনঃ নবায়ন হবে&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>string</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">string </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>name</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF008000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>="you_are_about_to_unsubscribe"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt;আপনি আনসাবস্ক্রাইব করতে যাচ্ছেন!&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>string</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">string </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>name</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF008000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>="msg_subscription_expired"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt;আপনার পূর্ববর্তী সাবস্ক্রিপশনের মেয়াদ শেষ হয়ে গেছে। দেখতে পুনরায় সাবস্ক্রাইব করুন&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>string</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">string </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>name</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF008000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>="button_view_plan"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt;প্ল্যান দেখুন&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>string</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">string </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>name</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF008000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>="title_trial_ending"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt;আপনার %s শেষ হতে চলেছে&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>string</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">string </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>name</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF008000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>="msg_invalid_email"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt;বৈধ ইমেল ঠিকানা লিখুন&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>string</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">string </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>name</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF008000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>="package_data_not_found"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt;কোন প্যাকেজ পাওয়া যায়নি&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>string</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">string </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>name</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF008000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>="pay_by_card"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt;কার্ড দিয়ে পে করুন&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>string</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">string </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>name</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF008000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>="pay_by_card_caps"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt;কার্ড দ্বারা পেমেন্ট&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>string</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">string </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>name</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF008000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>="continue_with_trial_plan"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt;ট্রায়াল প্ল্যান বজায় রাখুন&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>string</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">string </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>name</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF008000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>="choose_payment_method"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt;পেমেন্ট এর পদ্ধতি সিলেক্ট করুন&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>string</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">string </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>name</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF008000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>="title_subscribe_dialog"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt;ধন্যবাদ!&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>string</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">string </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>name</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF008000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>="enter_expire_msg"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt;মেয়াদ উত্তীর্ণ হবার তারিখ&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>string</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">string </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>name</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF008000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>="enter_cvc_number"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt;সিভিসি নম্বর লিখুন&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>string</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">string </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>name</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF008000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>="invalid_card_number"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt;ভুল কার্ড নাম্বার&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>string</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">string </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>name</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF008000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>="invalid_expire_date"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt;ভুল মেয়াদ উত্তীর্ণের তারিখ&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>string</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">string </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>name</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF008000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>="invalid_cvc_number"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt;ভুল সিভিসি নম্বর&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>string</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">string </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>name</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF008000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>="your_card_is_invalid"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt;আপনার কার্ডটি গ্রহণযোগ্য নয়&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>string</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">string </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>name</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF008000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>="msg_failed_to_check_subs_info"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt;সাবস্ক্রিপশন তথ্য পরীক্ষা করতে ব্যর্থ&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>string</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">string </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>name</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF008000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>="current_plan"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt;বর্তমান প্ল্যান&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>string</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">string </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>name</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF008000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>="if_you_are_sure_you_would_like_to_cancel_your_subscription_please_confirm_cancellation_will_be_effective_at_the_end_of_your_current_subscription_period_you_can_come_back_anytime_you_want"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt;দয়া করে আনসাবস্ক্রাইব এর ব্যাপারে নিশ্চিত হয়ে কনফার্ম করুন। আপনার বর্তমান প্ল্যান এর মেয়াদের পরে এই আনসাবস্ক্রাইব কার্যকর হবে। পরবর্তিতে যে কোন সময় আপনি আবার সাবস্ক্রাইব করতে পারবেন।&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>string</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">string </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>name</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF008000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>="congratulations"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt;অভিনন্দন&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>string</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">string </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>name</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF008000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>="you_ve_successfully_subscribed_to_your_selected_plan_and_you_have_been_charged_accordingly_you_can_un_subscribe_anytime_from_your_account_page"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt;চার্জিং সফল হয়েছে এবং আপনি আপনার সিলেক্ট করা প্ল্যান এ সাবস্ক্রাইব করেছেন। একাউন্ট পেজ থেকে যে কোন সময় আপনি আনসাবস্ক্রাইব করতে পারবেন।&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>string</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">string </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>name</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF008000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>="sorry"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt;দুঃখিত!&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>string</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">string </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>name</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF008000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>="your_subscription_process_has_failed"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt;আপনার সাবস্ক্রিপ্শন সফল হয়নি।&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>string</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">string </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>name</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF008000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>="confirm"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt;কনফার্ম করুন&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>string</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">string </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>name</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF008000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>="renew"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt;নবায়ন করুন&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>string</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">string </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>name</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF008000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>="have_a_promo_code"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt;প্রোমো কোড আছে?&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>string</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">string </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>name</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF008000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>="promo_code_applied_successfully"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt;পপ্রোমো কোড দেয়া সফল হয়েছে&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF000080"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>string</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>&gt;</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -2813,13 +5712,40 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-5000445]0"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF000080"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF0000FF"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF008000"/>
+      <name val="Menlo"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -2842,9 +5768,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3161,7 +6088,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A3F0CAB-B764-494E-8312-86738EB4583E}">
   <dimension ref="A1:C258"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="138" workbookViewId="0">
+    <sheetView zoomScale="138" workbookViewId="0">
       <selection activeCell="D247" sqref="D247"/>
     </sheetView>
   </sheetViews>
@@ -8763,4 +11690,249 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9C45ACD-84D1-2B4C-8B11-FDD5B344B611}">
+  <dimension ref="A1:A46"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="132" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45:A46"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>924</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>925</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>926</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>927</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>928</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>929</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>930</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>933</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>934</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>935</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>938</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>939</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>940</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>941</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>942</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>943</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>944</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
+        <v>946</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
+        <v>947</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
+        <v>948</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
+        <v>949</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
+        <v>950</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
+        <v>951</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
+        <v>952</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="s">
+        <v>953</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
+        <v>954</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="s">
+        <v>955</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" s="2" t="s">
+        <v>956</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" s="2" t="s">
+        <v>957</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35" s="2" t="s">
+        <v>958</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A36" s="2" t="s">
+        <v>959</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37" s="2" t="s">
+        <v>960</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A38" s="2" t="s">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A39" s="2" t="s">
+        <v>962</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A40" s="2" t="s">
+        <v>963</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A41" s="2" t="s">
+        <v>964</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A42" s="2" t="s">
+        <v>965</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A43" s="2" t="s">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A44" s="2" t="s">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A45" s="2" t="s">
+        <v>968</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A46" s="2" t="s">
+        <v>969</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update string database add sample data add arrays
</commit_message>
<xml_diff>
--- a/files/strings.xlsx
+++ b/files/strings.xlsx
@@ -8,16 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/storex/dLab/andStudio/lime-strings/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFFEAAC6-1D5E-E44E-AA81-46563111175E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6FD3DCF-9FB7-CE4F-BF01-D2F00AD8FECE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16240" xr2:uid="{2A2A4A0D-8F67-1149-8B79-481C2E1F4E29}"/>
+    <workbookView xWindow="28800" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="2" xr2:uid="{2A2A4A0D-8F67-1149-8B79-481C2E1F4E29}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId3"/>
-    <sheet name="Sheet5" sheetId="5" r:id="rId4"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId5"/>
+    <sheet name="main" sheetId="1" r:id="rId1"/>
+    <sheet name="number" sheetId="8" r:id="rId2"/>
+    <sheet name="dummy" sheetId="6" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId4"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId5"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId6"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1598" uniqueCount="1134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1658" uniqueCount="1201">
   <si>
     <t>bangla</t>
   </si>
@@ -3436,16 +3438,218 @@
   </si>
   <si>
     <t>active_plan_none</t>
+  </si>
+  <si>
+    <t>ইতোমধ্যে শেষ হয়ে গিয়েছে চলতি বিপিএলের ৭টি ম্যাচ। কিন্তু এখনো পর্যন্ত সে অর্থে বাংলাদেশের কেউই জ্বলে উঠতে পারেননি ব্যাট হাতে। বুধবার সবশেষ ম্যাচে তরুণ আফিফ হোসেন ধ্রুবর ৪৫ রানের ইনিংসটিই এখনো পর্যন্ত বাংলাদেশি ব্যাটসম্যানদের সেরা ইনিংস। এছাড়া ঢাকা ডায়নামাইটসের প্রথম ম্যাচে ১৪ বলে ৩৮ রানের তুফান চালিয়েছিলেন শুভাগত হোম।</t>
+  </si>
+  <si>
+    <t>চারিগ্রাম প্রাথমিক বিদ্যালয়</t>
+  </si>
+  <si>
+    <t>ইনাম আহমেদ</t>
+  </si>
+  <si>
+    <t>ফরিদা ইয়াসমিন</t>
+  </si>
+  <si>
+    <t>পরিদর্শক</t>
+  </si>
+  <si>
+    <t>ছড়া লেখা প্রতিযোগিতা</t>
+  </si>
+  <si>
+    <t>ইতোমধ্যে শেষ হয়ে গিয়েছে চলতি বিপিএলের ৭টি ম্যাচ। কিন্তু এখনো পর্যন্ত সে অর্থে বাংলাদেশের কেউই জ্বলে উঠতে পারেননি ব্যাট হাতে। বুধবার সবশেষ ম্যাচে তরুণ আফিফ হোসেন ধ্রুবর ৪৫ রানের ইনিংসটিই এখনো পর্যন্ত বাংলাদেশি ব্যাটসম্যানদের সেরা ইনিংস।</t>
+  </si>
+  <si>
+    <t>dummy_date_time</t>
+  </si>
+  <si>
+    <t>dummy_text_small</t>
+  </si>
+  <si>
+    <t>dummy_text_medium</t>
+  </si>
+  <si>
+    <t>dummy_text_big</t>
+  </si>
+  <si>
+    <t>Charigram High School</t>
+  </si>
+  <si>
+    <t>Inam Ahmed</t>
+  </si>
+  <si>
+    <t>Farida Yesmin</t>
+  </si>
+  <si>
+    <t>Inspector</t>
+  </si>
+  <si>
+    <t>Rhymes Contest</t>
+  </si>
+  <si>
+    <t>Sport includes all forms of competitive physical activity or games which, through casual or organised participation, aim to use, maintain or improve physical ability and skills while providing enjoyment to participants</t>
+  </si>
+  <si>
+    <t>Sport includes all forms of competitive physical activity or games which, through casual or organised participation</t>
+  </si>
+  <si>
+    <t>dummy_date</t>
+  </si>
+  <si>
+    <t>dummy_designation</t>
+  </si>
+  <si>
+    <t>dummy_mobile_no</t>
+  </si>
+  <si>
+    <t>dummy_name_female</t>
+  </si>
+  <si>
+    <t>dummy_name_male</t>
+  </si>
+  <si>
+    <t>dummy_name_school</t>
+  </si>
+  <si>
+    <t>num_0</t>
+  </si>
+  <si>
+    <t>num_1</t>
+  </si>
+  <si>
+    <t>num_2</t>
+  </si>
+  <si>
+    <t>num_3</t>
+  </si>
+  <si>
+    <t>num_4</t>
+  </si>
+  <si>
+    <t>num_5</t>
+  </si>
+  <si>
+    <t>num_6</t>
+  </si>
+  <si>
+    <t>num_7</t>
+  </si>
+  <si>
+    <t>num_8</t>
+  </si>
+  <si>
+    <t>num_9</t>
+  </si>
+  <si>
+    <t>zero</t>
+  </si>
+  <si>
+    <t>one</t>
+  </si>
+  <si>
+    <t>two</t>
+  </si>
+  <si>
+    <t>three</t>
+  </si>
+  <si>
+    <t>four</t>
+  </si>
+  <si>
+    <t>five</t>
+  </si>
+  <si>
+    <t>six</t>
+  </si>
+  <si>
+    <t>seven</t>
+  </si>
+  <si>
+    <t>eight</t>
+  </si>
+  <si>
+    <t>nine</t>
+  </si>
+  <si>
+    <t>শুন্য</t>
+  </si>
+  <si>
+    <t>এক</t>
+  </si>
+  <si>
+    <t>দুই</t>
+  </si>
+  <si>
+    <t>তিন</t>
+  </si>
+  <si>
+    <t>চার</t>
+  </si>
+  <si>
+    <t>পাঁচ</t>
+  </si>
+  <si>
+    <t>ছয়</t>
+  </si>
+  <si>
+    <t>সাত</t>
+  </si>
+  <si>
+    <t>আট</t>
+  </si>
+  <si>
+    <t>নয়</t>
+  </si>
+  <si>
+    <t>num_0_spl</t>
+  </si>
+  <si>
+    <t>num_1_spl</t>
+  </si>
+  <si>
+    <t>num_2_spl</t>
+  </si>
+  <si>
+    <t>num_3_spl</t>
+  </si>
+  <si>
+    <t>num_4_spl</t>
+  </si>
+  <si>
+    <t>num_5_spl</t>
+  </si>
+  <si>
+    <t>num_6_spl</t>
+  </si>
+  <si>
+    <t>num_7_spl</t>
+  </si>
+  <si>
+    <t>num_8_spl</t>
+  </si>
+  <si>
+    <t>num_9_spl</t>
+  </si>
+  <si>
+    <t>gps_open_confirmation</t>
+  </si>
+  <si>
+    <t>আপনি কি লোকেশন সার্ভিসটি অন করতে চান?</t>
+  </si>
+  <si>
+    <t>Do you want to open gps?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-5000445]0"/>
+    <numFmt numFmtId="167" formatCode="[$-5000000]dd/mm/yy"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -3472,6 +3676,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -3493,12 +3703,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3813,10 +4026,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A3F0CAB-B764-494E-8312-86738EB4583E}">
-  <dimension ref="A1:G302"/>
+  <dimension ref="A1:G300"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A291" zoomScale="138" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView zoomScale="138" workbookViewId="0">
+      <selection activeCell="B86" sqref="B86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4410,332 +4623,332 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>439</v>
-      </c>
-      <c r="B54">
-        <v>1834927083</v>
-      </c>
-      <c r="C54" s="1">
-        <v>1834548739</v>
+        <v>101</v>
+      </c>
+      <c r="B54" t="s">
+        <v>378</v>
+      </c>
+      <c r="C54" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>101</v>
+        <v>440</v>
       </c>
       <c r="B55" t="s">
-        <v>378</v>
+        <v>717</v>
       </c>
       <c r="C55" t="s">
-        <v>237</v>
+        <v>507</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
-        <v>440</v>
-      </c>
-      <c r="B56" t="s">
-        <v>717</v>
-      </c>
-      <c r="C56" t="s">
-        <v>507</v>
+      <c r="A56" s="2" t="s">
+        <v>1060</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>1024</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>919</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A57" s="2" t="s">
-        <v>1060</v>
-      </c>
-      <c r="B57" s="3" t="s">
-        <v>1024</v>
-      </c>
-      <c r="C57" s="3" t="s">
-        <v>919</v>
+      <c r="A57" t="s">
+        <v>28</v>
+      </c>
+      <c r="B57" t="s">
+        <v>301</v>
+      </c>
+      <c r="C57" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>28</v>
+        <v>2</v>
       </c>
       <c r="B58" t="s">
-        <v>301</v>
+        <v>275</v>
       </c>
       <c r="C58" t="s">
-        <v>158</v>
+        <v>131</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>2</v>
+        <v>73</v>
       </c>
       <c r="B59" t="s">
-        <v>275</v>
+        <v>344</v>
       </c>
       <c r="C59" t="s">
-        <v>131</v>
+        <v>203</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
-        <v>73</v>
-      </c>
-      <c r="B60" t="s">
-        <v>344</v>
-      </c>
-      <c r="C60" t="s">
-        <v>203</v>
+      <c r="A60" s="2" t="s">
+        <v>1030</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>1006</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>925</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
-        <v>1030</v>
+        <v>1032</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>1006</v>
+        <v>1009</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>925</v>
+        <v>928</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A62" s="2" t="s">
-        <v>1032</v>
-      </c>
-      <c r="B62" s="3" t="s">
-        <v>1009</v>
-      </c>
-      <c r="C62" s="3" t="s">
-        <v>928</v>
+      <c r="A62" t="s">
+        <v>782</v>
+      </c>
+      <c r="B62" t="s">
+        <v>783</v>
+      </c>
+      <c r="C62" t="s">
+        <v>508</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>782</v>
+        <v>104</v>
       </c>
       <c r="B63" t="s">
-        <v>783</v>
+        <v>381</v>
       </c>
       <c r="C63" t="s">
-        <v>508</v>
+        <v>240</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="B64" t="s">
-        <v>381</v>
+        <v>371</v>
       </c>
       <c r="C64" t="s">
-        <v>240</v>
+        <v>230</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>94</v>
+        <v>441</v>
       </c>
       <c r="B65" t="s">
-        <v>371</v>
+        <v>721</v>
       </c>
       <c r="C65" t="s">
-        <v>230</v>
+        <v>513</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="B66" t="s">
-        <v>721</v>
+        <v>723</v>
       </c>
       <c r="C66" t="s">
-        <v>513</v>
+        <v>142</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B67" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="C67" t="s">
-        <v>142</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>442</v>
+        <v>1083</v>
       </c>
       <c r="B68" t="s">
-        <v>722</v>
+        <v>764</v>
       </c>
       <c r="C68" t="s">
-        <v>1127</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>1083</v>
+        <v>11</v>
       </c>
       <c r="B69" t="s">
-        <v>764</v>
+        <v>284</v>
       </c>
       <c r="C69" t="s">
-        <v>1128</v>
+        <v>139</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>11</v>
+        <v>1061</v>
       </c>
       <c r="B70" t="s">
-        <v>284</v>
+        <v>843</v>
       </c>
       <c r="C70" t="s">
-        <v>139</v>
+        <v>844</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>1061</v>
+        <v>80</v>
       </c>
       <c r="B71" t="s">
-        <v>843</v>
+        <v>357</v>
       </c>
       <c r="C71" t="s">
-        <v>844</v>
+        <v>516</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>80</v>
+        <v>1108</v>
       </c>
       <c r="B72" t="s">
-        <v>357</v>
-      </c>
-      <c r="C72" t="s">
-        <v>516</v>
+        <v>1109</v>
+      </c>
+      <c r="C72" s="4" t="s">
+        <v>1107</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>1108</v>
+        <v>90</v>
       </c>
       <c r="B73" t="s">
-        <v>1109</v>
-      </c>
-      <c r="C73" s="4" t="s">
-        <v>1107</v>
+        <v>367</v>
+      </c>
+      <c r="C73" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>90</v>
+        <v>24</v>
       </c>
       <c r="B74" t="s">
-        <v>367</v>
+        <v>297</v>
       </c>
       <c r="C74" t="s">
-        <v>226</v>
+        <v>154</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>24</v>
+        <v>115</v>
       </c>
       <c r="B75" t="s">
-        <v>297</v>
+        <v>393</v>
       </c>
       <c r="C75" t="s">
-        <v>154</v>
+        <v>252</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>115</v>
+        <v>78</v>
       </c>
       <c r="B76" t="s">
-        <v>393</v>
+        <v>355</v>
       </c>
       <c r="C76" t="s">
-        <v>252</v>
+        <v>214</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>78</v>
+        <v>98</v>
       </c>
       <c r="B77" t="s">
-        <v>355</v>
+        <v>375</v>
       </c>
       <c r="C77" t="s">
-        <v>214</v>
+        <v>234</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>98</v>
+        <v>865</v>
       </c>
       <c r="B78" t="s">
-        <v>375</v>
+        <v>390</v>
       </c>
       <c r="C78" t="s">
-        <v>234</v>
+        <v>249</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>865</v>
+        <v>113</v>
       </c>
       <c r="B79" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="C79" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>113</v>
+        <v>3</v>
       </c>
       <c r="B80" t="s">
-        <v>391</v>
+        <v>276</v>
       </c>
       <c r="C80" t="s">
-        <v>250</v>
+        <v>132</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>3</v>
+        <v>886</v>
       </c>
       <c r="B81" t="s">
-        <v>276</v>
-      </c>
-      <c r="C81" t="s">
-        <v>132</v>
+        <v>887</v>
+      </c>
+      <c r="C81" s="4" t="s">
+        <v>1065</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>886</v>
+        <v>884</v>
       </c>
       <c r="B82" t="s">
-        <v>887</v>
+        <v>885</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>1065</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>884</v>
+        <v>1198</v>
       </c>
       <c r="B83" t="s">
-        <v>885</v>
-      </c>
-      <c r="C83" s="4" t="s">
-        <v>1066</v>
+        <v>1200</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>1199</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
@@ -6457,7 +6670,7 @@
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
-        <v>476</v>
+        <v>1113</v>
       </c>
       <c r="B242" t="s">
         <v>756</v>
@@ -6468,7 +6681,7 @@
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
-        <v>825</v>
+        <v>1114</v>
       </c>
       <c r="B243" t="s">
         <v>756</v>
@@ -6478,656 +6691,634 @@
       </c>
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A244" t="s">
-        <v>1113</v>
-      </c>
-      <c r="B244" t="s">
-        <v>756</v>
-      </c>
-      <c r="C244" t="s">
-        <v>554</v>
+      <c r="A244" s="2" t="s">
+        <v>905</v>
+      </c>
+      <c r="B244" s="3" t="s">
+        <v>978</v>
+      </c>
+      <c r="C244" s="3" t="s">
+        <v>932</v>
       </c>
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
-        <v>1114</v>
+        <v>84</v>
       </c>
       <c r="B245" t="s">
-        <v>756</v>
+        <v>361</v>
       </c>
       <c r="C245" t="s">
-        <v>555</v>
+        <v>219</v>
       </c>
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A246" s="2" t="s">
-        <v>905</v>
+        <v>897</v>
       </c>
       <c r="B246" s="3" t="s">
-        <v>978</v>
+        <v>975</v>
       </c>
       <c r="C246" s="3" t="s">
-        <v>932</v>
+        <v>911</v>
       </c>
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
-        <v>84</v>
+        <v>27</v>
       </c>
       <c r="B247" t="s">
-        <v>361</v>
+        <v>300</v>
       </c>
       <c r="C247" t="s">
-        <v>219</v>
+        <v>157</v>
       </c>
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A248" s="2" t="s">
-        <v>897</v>
-      </c>
-      <c r="B248" s="3" t="s">
-        <v>975</v>
-      </c>
-      <c r="C248" s="3" t="s">
-        <v>911</v>
+      <c r="A248" t="s">
+        <v>26</v>
+      </c>
+      <c r="B248" t="s">
+        <v>299</v>
+      </c>
+      <c r="C248" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
-        <v>27</v>
+        <v>1048</v>
       </c>
       <c r="B249" t="s">
-        <v>300</v>
+        <v>758</v>
       </c>
       <c r="C249" t="s">
-        <v>157</v>
+        <v>557</v>
       </c>
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A250" t="s">
-        <v>26</v>
-      </c>
-      <c r="B250" t="s">
-        <v>299</v>
-      </c>
-      <c r="C250" t="s">
-        <v>156</v>
+      <c r="A250" s="2" t="s">
+        <v>1041</v>
+      </c>
+      <c r="B250" s="3" t="s">
+        <v>996</v>
+      </c>
+      <c r="C250" s="3" t="s">
+        <v>917</v>
       </c>
     </row>
     <row r="251" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A251" t="s">
-        <v>1048</v>
-      </c>
-      <c r="B251" t="s">
-        <v>758</v>
-      </c>
-      <c r="C251" t="s">
-        <v>557</v>
+      <c r="A251" s="2" t="s">
+        <v>1035</v>
+      </c>
+      <c r="B251" s="3" t="s">
+        <v>1045</v>
+      </c>
+      <c r="C251" s="3" t="s">
+        <v>1044</v>
       </c>
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A252" s="2" t="s">
-        <v>1041</v>
+        <v>1042</v>
       </c>
       <c r="B252" s="3" t="s">
-        <v>996</v>
+        <v>1043</v>
       </c>
       <c r="C252" s="3" t="s">
-        <v>917</v>
+        <v>918</v>
       </c>
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A253" s="2" t="s">
-        <v>1035</v>
-      </c>
-      <c r="B253" s="3" t="s">
-        <v>1045</v>
-      </c>
-      <c r="C253" s="3" t="s">
-        <v>1044</v>
+      <c r="A253" t="s">
+        <v>1047</v>
+      </c>
+      <c r="B253" t="s">
+        <v>757</v>
+      </c>
+      <c r="C253" t="s">
+        <v>556</v>
       </c>
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A254" s="2" t="s">
-        <v>1042</v>
+        <v>1047</v>
       </c>
       <c r="B254" s="3" t="s">
-        <v>1043</v>
+        <v>1015</v>
       </c>
       <c r="C254" s="3" t="s">
-        <v>918</v>
+        <v>933</v>
       </c>
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A255" t="s">
-        <v>1047</v>
-      </c>
-      <c r="B255" t="s">
-        <v>757</v>
-      </c>
-      <c r="C255" t="s">
-        <v>556</v>
+      <c r="A255" s="2" t="s">
+        <v>1115</v>
+      </c>
+      <c r="B255" s="3" t="s">
+        <v>1037</v>
+      </c>
+      <c r="C255" s="3" t="s">
+        <v>1036</v>
       </c>
     </row>
     <row r="256" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A256" s="2" t="s">
-        <v>1047</v>
-      </c>
-      <c r="B256" s="3" t="s">
-        <v>1015</v>
-      </c>
-      <c r="C256" s="3" t="s">
-        <v>933</v>
+      <c r="A256" t="s">
+        <v>1038</v>
+      </c>
+      <c r="B256" t="s">
+        <v>759</v>
+      </c>
+      <c r="C256" t="s">
+        <v>558</v>
       </c>
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A257" s="2" t="s">
-        <v>1115</v>
-      </c>
-      <c r="B257" s="3" t="s">
-        <v>1037</v>
-      </c>
-      <c r="C257" s="3" t="s">
-        <v>1036</v>
+      <c r="A257" t="s">
+        <v>773</v>
+      </c>
+      <c r="B257" t="s">
+        <v>774</v>
+      </c>
+      <c r="C257" t="s">
+        <v>492</v>
       </c>
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
-        <v>1038</v>
+        <v>477</v>
       </c>
       <c r="B258" t="s">
-        <v>759</v>
+        <v>760</v>
       </c>
       <c r="C258" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
     </row>
     <row r="259" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
-        <v>773</v>
+        <v>1076</v>
       </c>
       <c r="B259" t="s">
-        <v>774</v>
+        <v>757</v>
       </c>
       <c r="C259" t="s">
-        <v>492</v>
+        <v>556</v>
       </c>
     </row>
     <row r="260" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
-        <v>477</v>
+        <v>1077</v>
       </c>
       <c r="B260" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="C260" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
-        <v>1076</v>
+        <v>1078</v>
       </c>
       <c r="B261" t="s">
-        <v>757</v>
+        <v>759</v>
       </c>
       <c r="C261" t="s">
-        <v>556</v>
+        <v>558</v>
       </c>
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
-        <v>1077</v>
+        <v>20</v>
       </c>
       <c r="B262" t="s">
-        <v>758</v>
+        <v>293</v>
       </c>
       <c r="C262" t="s">
-        <v>557</v>
+        <v>149</v>
       </c>
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A263" t="s">
-        <v>1078</v>
+        <v>120</v>
       </c>
       <c r="B263" t="s">
-        <v>759</v>
+        <v>398</v>
       </c>
       <c r="C263" t="s">
-        <v>558</v>
+        <v>257</v>
       </c>
     </row>
     <row r="264" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A264" t="s">
-        <v>20</v>
+        <v>812</v>
       </c>
       <c r="B264" t="s">
-        <v>293</v>
+        <v>813</v>
       </c>
       <c r="C264" t="s">
-        <v>149</v>
+        <v>840</v>
       </c>
     </row>
     <row r="265" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A265" t="s">
-        <v>120</v>
+        <v>97</v>
       </c>
       <c r="B265" t="s">
-        <v>398</v>
+        <v>374</v>
       </c>
       <c r="C265" t="s">
-        <v>257</v>
+        <v>233</v>
       </c>
     </row>
     <row r="266" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A266" t="s">
-        <v>812</v>
-      </c>
-      <c r="B266" t="s">
-        <v>813</v>
-      </c>
-      <c r="C266" t="s">
-        <v>840</v>
+      <c r="A266" s="2" t="s">
+        <v>1027</v>
+      </c>
+      <c r="B266" s="3" t="s">
+        <v>1028</v>
+      </c>
+      <c r="C266" s="3" t="s">
+        <v>924</v>
       </c>
     </row>
     <row r="267" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A267" t="s">
-        <v>97</v>
+        <v>50</v>
       </c>
       <c r="B267" t="s">
-        <v>374</v>
+        <v>324</v>
       </c>
       <c r="C267" t="s">
-        <v>233</v>
+        <v>179</v>
       </c>
     </row>
     <row r="268" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A268" s="2" t="s">
-        <v>1027</v>
-      </c>
-      <c r="B268" s="3" t="s">
-        <v>1028</v>
-      </c>
-      <c r="C268" s="3" t="s">
-        <v>924</v>
+      <c r="A268" t="s">
+        <v>47</v>
+      </c>
+      <c r="B268" t="s">
+        <v>321</v>
+      </c>
+      <c r="C268" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="269" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A269" t="s">
-        <v>50</v>
+        <v>892</v>
       </c>
       <c r="B269" t="s">
-        <v>324</v>
+        <v>332</v>
       </c>
       <c r="C269" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
     </row>
     <row r="270" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A270" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="B270" t="s">
-        <v>321</v>
+        <v>360</v>
       </c>
       <c r="C270" t="s">
-        <v>176</v>
+        <v>218</v>
       </c>
     </row>
     <row r="271" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A271" t="s">
-        <v>892</v>
-      </c>
-      <c r="B271" t="s">
-        <v>332</v>
-      </c>
-      <c r="C271" t="s">
-        <v>187</v>
+      <c r="A271" s="2" t="s">
+        <v>1025</v>
+      </c>
+      <c r="B271" s="3" t="s">
+        <v>1004</v>
+      </c>
+      <c r="C271" s="3" t="s">
+        <v>922</v>
       </c>
     </row>
     <row r="272" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A272" t="s">
-        <v>83</v>
+        <v>420</v>
       </c>
       <c r="B272" t="s">
-        <v>360</v>
+        <v>421</v>
       </c>
       <c r="C272" t="s">
-        <v>218</v>
+        <v>563</v>
       </c>
     </row>
     <row r="273" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A273" s="2" t="s">
-        <v>1025</v>
-      </c>
-      <c r="B273" s="3" t="s">
-        <v>1004</v>
-      </c>
-      <c r="C273" s="3" t="s">
-        <v>922</v>
+      <c r="A273" t="s">
+        <v>872</v>
+      </c>
+      <c r="B273" t="s">
+        <v>347</v>
+      </c>
+      <c r="C273" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="274" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A274" t="s">
-        <v>420</v>
+        <v>1116</v>
       </c>
       <c r="B274" t="s">
-        <v>421</v>
+        <v>348</v>
       </c>
       <c r="C274" t="s">
-        <v>563</v>
+        <v>207</v>
       </c>
     </row>
     <row r="275" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A275" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="B275" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="C275" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
     <row r="276" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A276" t="s">
-        <v>1116</v>
-      </c>
-      <c r="B276" t="s">
-        <v>348</v>
-      </c>
-      <c r="C276" t="s">
-        <v>207</v>
+      <c r="A276" s="2" t="s">
+        <v>982</v>
+      </c>
+      <c r="B276" s="3" t="s">
+        <v>983</v>
+      </c>
+      <c r="C276" s="3" t="s">
+        <v>910</v>
       </c>
     </row>
     <row r="277" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A277" t="s">
-        <v>873</v>
-      </c>
-      <c r="B277" t="s">
-        <v>349</v>
-      </c>
-      <c r="C277" t="s">
-        <v>208</v>
+      <c r="A277" s="2" t="s">
+        <v>1046</v>
+      </c>
+      <c r="B277" s="3" t="s">
+        <v>985</v>
+      </c>
+      <c r="C277" s="3" t="s">
+        <v>914</v>
       </c>
     </row>
     <row r="278" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A278" s="2" t="s">
-        <v>982</v>
-      </c>
-      <c r="B278" s="3" t="s">
-        <v>983</v>
-      </c>
-      <c r="C278" s="3" t="s">
-        <v>910</v>
+      <c r="A278" t="s">
+        <v>775</v>
+      </c>
+      <c r="B278" t="s">
+        <v>776</v>
+      </c>
+      <c r="C278" t="s">
+        <v>493</v>
       </c>
     </row>
     <row r="279" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A279" s="2" t="s">
-        <v>1046</v>
-      </c>
-      <c r="B279" s="3" t="s">
-        <v>985</v>
-      </c>
-      <c r="C279" s="3" t="s">
-        <v>914</v>
+      <c r="A279" t="s">
+        <v>41</v>
+      </c>
+      <c r="B279" t="s">
+        <v>314</v>
+      </c>
+      <c r="C279" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="280" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A280" t="s">
-        <v>775</v>
+        <v>479</v>
       </c>
       <c r="B280" t="s">
-        <v>776</v>
+        <v>762</v>
       </c>
       <c r="C280" t="s">
-        <v>493</v>
+        <v>808</v>
       </c>
     </row>
     <row r="281" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A281" t="s">
-        <v>41</v>
+        <v>63</v>
       </c>
       <c r="B281" t="s">
-        <v>314</v>
+        <v>340</v>
       </c>
       <c r="C281" t="s">
-        <v>169</v>
+        <v>193</v>
       </c>
     </row>
     <row r="282" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A282" t="s">
-        <v>479</v>
+        <v>64</v>
       </c>
       <c r="B282" t="s">
-        <v>762</v>
+        <v>341</v>
       </c>
       <c r="C282" t="s">
-        <v>808</v>
+        <v>194</v>
       </c>
     </row>
     <row r="283" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A283" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B283" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="C283" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
     </row>
     <row r="284" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A284" t="s">
-        <v>64</v>
+        <v>9</v>
       </c>
       <c r="B284" t="s">
-        <v>341</v>
+        <v>282</v>
       </c>
       <c r="C284" t="s">
-        <v>194</v>
+        <v>137</v>
       </c>
     </row>
     <row r="285" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A285" t="s">
-        <v>65</v>
+        <v>1119</v>
       </c>
       <c r="B285" t="s">
-        <v>342</v>
+        <v>850</v>
       </c>
       <c r="C285" t="s">
-        <v>195</v>
+        <v>894</v>
       </c>
     </row>
     <row r="286" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A286" t="s">
-        <v>9</v>
+        <v>34</v>
       </c>
       <c r="B286" t="s">
-        <v>282</v>
+        <v>307</v>
       </c>
       <c r="C286" t="s">
-        <v>137</v>
+        <v>163</v>
       </c>
     </row>
     <row r="287" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A287" t="s">
-        <v>1119</v>
+        <v>828</v>
       </c>
       <c r="B287" t="s">
-        <v>850</v>
+        <v>829</v>
       </c>
       <c r="C287" t="s">
-        <v>894</v>
+        <v>836</v>
       </c>
     </row>
     <row r="288" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A288" t="s">
-        <v>34</v>
+        <v>859</v>
       </c>
       <c r="B288" t="s">
-        <v>307</v>
+        <v>835</v>
       </c>
       <c r="C288" t="s">
-        <v>163</v>
+        <v>837</v>
       </c>
     </row>
     <row r="289" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A289" t="s">
-        <v>828</v>
+        <v>868</v>
       </c>
       <c r="B289" t="s">
-        <v>829</v>
+        <v>831</v>
       </c>
       <c r="C289" t="s">
-        <v>836</v>
+        <v>838</v>
       </c>
     </row>
     <row r="290" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A290" t="s">
-        <v>859</v>
+        <v>1069</v>
       </c>
       <c r="B290" t="s">
-        <v>835</v>
+        <v>1070</v>
       </c>
       <c r="C290" t="s">
-        <v>837</v>
+        <v>521</v>
       </c>
     </row>
     <row r="291" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A291" t="s">
-        <v>868</v>
+        <v>803</v>
       </c>
       <c r="B291" t="s">
-        <v>831</v>
+        <v>804</v>
       </c>
       <c r="C291" t="s">
-        <v>838</v>
+        <v>565</v>
       </c>
     </row>
     <row r="292" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A292" t="s">
-        <v>1069</v>
+        <v>480</v>
       </c>
       <c r="B292" t="s">
-        <v>1070</v>
+        <v>763</v>
       </c>
       <c r="C292" t="s">
-        <v>521</v>
+        <v>566</v>
       </c>
     </row>
     <row r="293" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A293" t="s">
-        <v>803</v>
+        <v>801</v>
       </c>
       <c r="B293" t="s">
-        <v>804</v>
+        <v>802</v>
       </c>
       <c r="C293" t="s">
-        <v>565</v>
+        <v>567</v>
       </c>
     </row>
     <row r="294" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A294" t="s">
-        <v>480</v>
+        <v>1091</v>
       </c>
       <c r="B294" t="s">
-        <v>763</v>
+        <v>735</v>
       </c>
       <c r="C294" t="s">
-        <v>566</v>
+        <v>535</v>
       </c>
     </row>
     <row r="295" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A295" t="s">
-        <v>801</v>
+        <v>1067</v>
       </c>
       <c r="B295" t="s">
-        <v>802</v>
+        <v>1068</v>
       </c>
       <c r="C295" t="s">
-        <v>567</v>
+        <v>520</v>
       </c>
     </row>
     <row r="296" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A296" t="s">
-        <v>1091</v>
+        <v>32</v>
       </c>
       <c r="B296" t="s">
-        <v>735</v>
+        <v>305</v>
       </c>
       <c r="C296" t="s">
-        <v>535</v>
+        <v>161</v>
       </c>
     </row>
     <row r="297" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A297" t="s">
-        <v>1067</v>
+        <v>810</v>
       </c>
       <c r="B297" t="s">
-        <v>1068</v>
+        <v>811</v>
       </c>
       <c r="C297" t="s">
-        <v>520</v>
+        <v>564</v>
       </c>
     </row>
     <row r="298" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A298" t="s">
-        <v>32</v>
+        <v>481</v>
       </c>
       <c r="B298" t="s">
-        <v>305</v>
+        <v>569</v>
       </c>
       <c r="C298" t="s">
-        <v>161</v>
+        <v>569</v>
       </c>
     </row>
     <row r="299" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A299" t="s">
-        <v>810</v>
+        <v>109</v>
       </c>
       <c r="B299" t="s">
-        <v>811</v>
+        <v>386</v>
       </c>
       <c r="C299" t="s">
-        <v>564</v>
+        <v>245</v>
       </c>
     </row>
     <row r="300" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A300" t="s">
-        <v>481</v>
+        <v>14</v>
       </c>
       <c r="B300" t="s">
-        <v>569</v>
+        <v>287</v>
       </c>
       <c r="C300" t="s">
-        <v>569</v>
-      </c>
-    </row>
-    <row r="301" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A301" t="s">
-        <v>109</v>
-      </c>
-      <c r="B301" t="s">
-        <v>386</v>
-      </c>
-      <c r="C301" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="302" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A302" t="s">
-        <v>14</v>
-      </c>
-      <c r="B302" t="s">
-        <v>287</v>
-      </c>
-      <c r="C302" t="s">
         <v>143</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A1:C302">
+  <sortState ref="A1:C300">
     <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7135,11 +7326,387 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCEA4152-B241-2B40-986A-12C65FDBD0D0}">
+  <dimension ref="A1:G22"/>
+  <sheetViews>
+    <sheetView zoomScale="137" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>1158</v>
+      </c>
+      <c r="B1">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>1159</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>1160</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>1161</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>1162</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>1163</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>1164</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>1165</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>1166</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>1167</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="2"/>
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="2"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>1188</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1168</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>1178</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>1189</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1169</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>1179</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>1190</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1170</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>1180</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>1191</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1171</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>1181</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>1192</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1172</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>1182</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>1193</v>
+      </c>
+      <c r="B18" t="s">
+        <v>1173</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>1183</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>1194</v>
+      </c>
+      <c r="B19" t="s">
+        <v>1174</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>1184</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>1195</v>
+      </c>
+      <c r="B20" t="s">
+        <v>1175</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>1185</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>1196</v>
+      </c>
+      <c r="B21" t="s">
+        <v>1176</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>1186</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
+        <v>1197</v>
+      </c>
+      <c r="B22" t="s">
+        <v>1177</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>1187</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57E8B14F-D8DF-7442-B880-5BE5847F9131}">
+  <dimension ref="A1:C18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="132" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="32.33203125" customWidth="1"/>
+    <col min="3" max="3" width="34.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>1152</v>
+      </c>
+      <c r="B1" s="7">
+        <v>43059</v>
+      </c>
+      <c r="C1" s="5">
+        <v>43059</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>1141</v>
+      </c>
+      <c r="B2" s="6">
+        <v>43496.627465277779</v>
+      </c>
+      <c r="C2" s="6">
+        <v>43496.627465277779</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>1153</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>1148</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1138</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>1154</v>
+      </c>
+      <c r="B4" s="2">
+        <v>1731487887</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1731487887</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>1155</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>1147</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1137</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>1156</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>1146</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1136</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>1157</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>1145</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1135</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>1144</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>1150</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>1134</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>1143</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>1151</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1140</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>1142</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>1149</v>
+      </c>
+      <c r="C10" t="s">
+        <v>1139</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B18" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21CF7B10-8A83-C844-9233-3895305C52AA}">
   <dimension ref="A1:C116"/>
   <sheetViews>
     <sheetView zoomScale="125" workbookViewId="0">
-      <selection activeCell="A13" sqref="A1:C116"/>
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8412,7 +8979,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9C45ACD-84D1-2B4C-8B11-FDD5B344B611}">
   <dimension ref="A1:C36"/>
   <sheetViews>
@@ -8828,7 +9395,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{690C5D52-6B15-194B-A1ED-FBFB6A1C3A43}">
   <dimension ref="A1:G46"/>
   <sheetViews>
@@ -9402,7 +9969,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1ED7931A-D0A1-A744-A873-C9F6059F675B}">
   <dimension ref="A1:B166"/>
   <sheetViews>

</xml_diff>